<commit_message>
Modifique y borre archivos
</commit_message>
<xml_diff>
--- a/Calculo_Mon.xlsx
+++ b/Calculo_Mon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Mi_destino_Montero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Mi_Destino_Montero\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Càlculo de nota</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Pràctica</t>
+  </si>
+  <si>
+    <t>hollllaaaaaaaaaaaaaaaa</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E9"/>
+  <dimension ref="B4:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,6 +452,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>